<commit_message>
Update Modelado de dominio enriquecido.xlsx
</commit_message>
<xml_diff>
--- a/Clase/Modelo de dominio/Modelado de dominio enriquecido.xlsx
+++ b/Clase/Modelo de dominio/Modelado de dominio enriquecido.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddfc1a2aaa1b6043/Documentos/GitHub/Presupuesto/Clase/Modelo de dominio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{C43FD99A-738B-4C32-8F0D-7948FDBB67D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EF5FF1B-3AD1-49A0-AD0E-D9CA187508AE}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{C43FD99A-738B-4C32-8F0D-7948FDBB67D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{356FD2A6-5B9F-412A-BE18-DF9469DBF66B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="657" firstSheet="2" activeTab="6" xr2:uid="{40064D5F-B35F-41F3-A50B-554BD813C67A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="657" firstSheet="3" activeTab="7" xr2:uid="{40064D5F-B35F-41F3-A50B-554BD813C67A}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Tipo Rubro- Datos Simulados" sheetId="6" r:id="rId5"/>
     <sheet name="Rubro" sheetId="5" r:id="rId6"/>
     <sheet name="Tipo Identificacion" sheetId="7" r:id="rId7"/>
+    <sheet name="Tipo Identificacion-Datos Simul" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>Tipo de Dato</t>
   </si>
@@ -290,6 +291,27 @@
   </si>
   <si>
     <t>No es posible tener masde un tipo de identificacion con el mismo nombre</t>
+  </si>
+  <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>Tipo de identificacion que sirve para asociarlo a las personas mayores de edady que ya han sacado si cedula</t>
+  </si>
+  <si>
+    <t>Cedula Extranjeria</t>
+  </si>
+  <si>
+    <t>Numero de identificacion personal</t>
+  </si>
+  <si>
+    <t>Identificacion Tibutaria</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>Tarjeta de identidad</t>
   </si>
 </sst>
 </file>
@@ -376,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -421,6 +443,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -439,22 +479,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1154,72 +1179,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>'Objetos de Dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="18" t="str">
+      <c r="B2" s="24" t="str">
         <f>'Objetos de Dominio'!A2</f>
         <v>Tipo Rubro</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" s="8" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="str">
         <f>'Objetos de Dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="19" t="str">
+      <c r="B3" s="25" t="str">
         <f>'Objetos de Dominio'!$B$2</f>
         <v>Entidad que representa un tipo de rubro, el cual corresponde a la categoria a la cual pertence un rubro determinado o un compromiso financiero. Por ejemplo un tipo de rubro  puede ser ingreso, el cual indica que los rubros catagorizados con él, corresponde a dinero que la persona va a recibir por diferentes razones: salarios ,inversiones, ganancias ocacionales</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -1473,10 +1498,10 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="27" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1490,8 +1515,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="10" t="s">
         <v>63</v>
       </c>
@@ -1598,7 +1623,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,24 +1633,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="str">
@@ -1812,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F44EA2-F196-4F9F-A7F8-D22ADEEA91C2}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
@@ -1837,75 +1862,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
     </row>
     <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="str">
         <f>'Objetos de Dominio'!$A$1&amp;":"</f>
         <v>Objeto de Dominio:</v>
       </c>
-      <c r="B2" s="19" t="str">
+      <c r="B2" s="25" t="str">
         <f>'Objetos de Dominio'!A2</f>
         <v>Tipo Rubro</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="str">
         <f>'Objetos de Dominio'!$B$1&amp;":"</f>
         <v>Descripción:</v>
       </c>
-      <c r="B3" s="19" t="str">
+      <c r="B3" s="25" t="str">
         <f>'Objetos de Dominio'!$B$2</f>
         <v>Entidad que representa un tipo de rubro, el cual corresponde a la categoria a la cual pertence un rubro determinado o un compromiso financiero. Por ejemplo un tipo de rubro  puede ser ingreso, el cual indica que los rubros catagorizados con él, corresponde a dinero que la persona va a recibir por diferentes razones: salarios ,inversiones, ganancias ocacionales</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>72</v>
       </c>
       <c r="B4" s="8"/>
@@ -1925,7 +1950,7 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1975,48 +2000,48 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="19">
         <v>10</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="19">
         <v>10</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25" t="s">
+      <c r="I6" s="19"/>
+      <c r="J6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="25" t="s">
+      <c r="O6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="P6" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>28</v>
       </c>
@@ -2057,44 +2082,44 @@
       <c r="P7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-    </row>
-    <row r="8" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-    </row>
-    <row r="9" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+    </row>
+    <row r="8" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+    </row>
+    <row r="9" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
     </row>
     <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -2120,10 +2145,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="27" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -2131,8 +2156,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="10" t="s">
         <v>63</v>
       </c>
@@ -2171,4 +2196,133 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B9D1DF-C9BD-4E54-B8A3-D913FB05DB72}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="str">
+        <f>'Tipo Rubro'!$A$6</f>
+        <v>Identificador</v>
+      </c>
+      <c r="B2" s="29" t="str">
+        <f>'Tipo Rubro'!$A$7</f>
+        <v>Nombre</v>
+      </c>
+      <c r="C2" s="15" t="str">
+        <f>'Tipo Rubro'!$A$8</f>
+        <v>Descripcion</v>
+      </c>
+      <c r="D2" s="15" t="str">
+        <f>'Tipo Rubro'!$A$9</f>
+        <v>Estado</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Tipo Rubro'!A6" display="'Tipo Rubro'!A6" xr:uid="{98E25BF8-62EC-418E-9AD4-F090776A36DA}"/>
+    <hyperlink ref="B2" location="'Tipo Rubro'!A7" display="'Tipo Rubro'!A7" xr:uid="{F473D5C9-05AB-4D8B-B0F9-968CDED2DE95}"/>
+    <hyperlink ref="C2" location="'Tipo Rubro'!A8" display="'Tipo Rubro'!A8" xr:uid="{BB2E1AAA-06D9-452F-9FBB-C78C1B981386}"/>
+    <hyperlink ref="D2" location="'Tipo Rubro'!A9" display="'Tipo Rubro'!A9" xr:uid="{C2CAA311-1A98-488B-9CEB-CA0D5DFD6061}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al Inicio" xr:uid="{F0D5C8AD-EEE5-4374-A897-6F97CF494000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B8B79FC6-86C3-4F56-A2B8-003F3362BEE1}">
+          <x14:formula1>
+            <xm:f>Valores!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>